<commit_message>
Updated test scripts and resources
</commit_message>
<xml_diff>
--- a/src/test/resources/adscreateandedit.xlsx
+++ b/src/test/resources/adscreateandedit.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E8EF84C4-D5E5-401E-8B2D-D3A36EB9ED85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13580" windowHeight="4170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
     <sheet name="edit" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -139,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,28 +457,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.90625" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,7 +511,7 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -553,37 +550,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" customWidth="1"/>
-    <col min="15" max="15" width="19.21875" customWidth="1"/>
-    <col min="16" max="16" width="16.21875" customWidth="1"/>
-    <col min="17" max="17" width="20.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="10.36328125" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="15" max="15" width="19.1796875" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" customWidth="1"/>
+    <col min="17" max="17" width="20.1796875" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="31.77734375" customWidth="1"/>
-    <col min="20" max="20" width="18.33203125" customWidth="1"/>
+    <col min="19" max="19" width="31.81640625" customWidth="1"/>
+    <col min="20" max="20" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -645,7 +642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>